<commit_message>
fix XR 11 size
why big widget h != w
</commit_message>
<xml_diff>
--- a/WidgetSizes.xlsx
+++ b/WidgetSizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Documents/GitHub/Transparency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170A84C2-E6E5-5147-9F15-A8D16AE058C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA1AD5-9ED8-8243-9ED3-A54A0ACD00BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18860" yWindow="4980" windowWidth="20360" windowHeight="17440" xr2:uid="{CFDEA34E-4ACB-A44B-ABA9-F104A4CF8651}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>设备</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,10 @@
   </si>
   <si>
     <t>3y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XR 360*379</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869A3B0C-F175-404E-8267-F1D4725AECD3}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1022,7 +1026,7 @@
         <v>169</v>
       </c>
       <c r="F9">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="H9">
         <v>80</v>
@@ -1227,6 +1231,9 @@
       </c>
     </row>
     <row r="16" spans="1:14">
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
       <c r="K16" t="s">
         <v>23</v>
       </c>

</xml_diff>